<commit_message>
version test read ok
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,11 +15,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Noms des applications</t>
   </si>
   <si>
+    <t>Prix</t>
+  </si>
+  <si>
     <t>test</t>
   </si>
   <si>
@@ -27,6 +30,15 @@
   </si>
   <si>
     <t>cest pas A3</t>
+  </si>
+  <si>
+    <t>Lieu</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t>Lile</t>
   </si>
 </sst>
 </file>
@@ -362,7 +374,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -370,28 +382,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>19745</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1475621</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:3">
       <c r="A5"/>
+      <c r="B5">
+        <v>834548</v>
+      </c>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>